<commit_message>
2.07-- bugfix alpha release
</commit_message>
<xml_diff>
--- a/doc/acl_decoder.xlsx
+++ b/doc/acl_decoder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsneed/Bobware/git/pwalk/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CEE8D2-7280-BE4D-966F-0B39D0A6614F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76766C8-5675-6549-957C-3C80EAD0C15B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="348">
   <si>
     <t>r</t>
   </si>
@@ -1432,6 +1432,9 @@
   </si>
   <si>
     <t>Windows compact form (ICACLS, etc)</t>
+  </si>
+  <si>
+    <t>delete_child (dir)</t>
   </si>
 </sst>
 </file>
@@ -4165,8 +4168,8 @@
   <dimension ref="A1:AH192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="3" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10124,7 +10127,7 @@
     </row>
     <row r="129" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="68" t="s">
-        <v>216</v>
+        <v>347</v>
       </c>
       <c r="B129" s="97" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
New xacls -s1 feature
</commit_message>
<xml_diff>
--- a/doc/acl_decoder.xlsx
+++ b/doc/acl_decoder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsneed/Bobware/git/pwalk/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9CBCED-4A78-2E45-BABB-ECB0C2A91EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C06E91-551D-0B44-9CC7-BB895075FE25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1220,9 +1220,6 @@
   </si>
   <si>
     <t>OneFS &amp; NFS4 keywords for 'Generic' bitmasks (compared with similar NFS4 masks) …</t>
-  </si>
-  <si>
-    <t>&lt;&lt;&lt; OS X mappings &gt;&gt;&gt;</t>
   </si>
   <si>
     <t>&lt;&lt;&lt; ZFS mappings (UNVALIDATED) &gt;&gt;&gt;</t>
@@ -1435,6 +1432,9 @@
   </si>
   <si>
     <t>write</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt; OSX/macOS mappings &gt;&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -4180,8 +4180,8 @@
   <dimension ref="A1:AH192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
+      <pane ySplit="3" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4197,7 +4197,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="290" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" s="291"/>
       <c r="C1" s="210">
@@ -4399,7 +4399,7 @@
     </row>
     <row r="3" spans="1:34" s="267" customFormat="1" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="268" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B3" s="269" t="s">
         <v>178</v>
@@ -4416,19 +4416,19 @@
       <c r="L3" s="271"/>
       <c r="M3" s="271"/>
       <c r="N3" s="273" t="s">
+        <v>299</v>
+      </c>
+      <c r="O3" s="270" t="s">
         <v>300</v>
       </c>
-      <c r="O3" s="270" t="s">
+      <c r="P3" s="271" t="s">
         <v>301</v>
       </c>
-      <c r="P3" s="271" t="s">
+      <c r="Q3" s="271" t="s">
         <v>302</v>
       </c>
-      <c r="Q3" s="271" t="s">
+      <c r="R3" s="272" t="s">
         <v>303</v>
-      </c>
-      <c r="R3" s="272" t="s">
-        <v>304</v>
       </c>
       <c r="S3" s="274"/>
       <c r="T3" s="275"/>
@@ -4436,37 +4436,37 @@
       <c r="V3" s="276"/>
       <c r="W3" s="274"/>
       <c r="X3" s="275" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y3" s="277" t="s">
         <v>305</v>
       </c>
-      <c r="Y3" s="277" t="s">
+      <c r="Z3" s="272" t="s">
         <v>306</v>
       </c>
-      <c r="Z3" s="272" t="s">
+      <c r="AA3" s="270" t="s">
         <v>307</v>
       </c>
-      <c r="AA3" s="270" t="s">
+      <c r="AB3" s="271" t="s">
         <v>308</v>
       </c>
-      <c r="AB3" s="271" t="s">
+      <c r="AC3" s="271" t="s">
         <v>309</v>
       </c>
-      <c r="AC3" s="271" t="s">
+      <c r="AD3" s="272" t="s">
         <v>310</v>
       </c>
-      <c r="AD3" s="272" t="s">
+      <c r="AE3" s="270" t="s">
         <v>311</v>
       </c>
-      <c r="AE3" s="270" t="s">
+      <c r="AF3" s="271" t="s">
         <v>312</v>
       </c>
-      <c r="AF3" s="271" t="s">
+      <c r="AG3" s="271" t="s">
         <v>313</v>
       </c>
-      <c r="AG3" s="271" t="s">
+      <c r="AH3" s="278" t="s">
         <v>314</v>
-      </c>
-      <c r="AH3" s="278" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:34" s="20" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
     </row>
     <row r="5" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="132" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B5" s="133"/>
       <c r="C5" s="118"/>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="7" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="77" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B7" s="88"/>
       <c r="C7" s="78"/>
@@ -4649,10 +4649,10 @@
       <c r="V7" s="156"/>
       <c r="W7" s="155"/>
       <c r="X7" s="156" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Y7" s="156" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Z7" s="81" t="s">
         <v>135</v>
@@ -4754,7 +4754,7 @@
     </row>
     <row r="9" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="237" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B9" s="238"/>
       <c r="C9" s="239"/>
@@ -4860,7 +4860,7 @@
     </row>
     <row r="11" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B11" s="133"/>
       <c r="C11" s="118"/>
@@ -5447,7 +5447,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="34"/>
@@ -6270,7 +6270,7 @@
     </row>
     <row r="43" spans="1:34" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="136" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B43" s="114"/>
       <c r="C43" s="113"/>
@@ -6312,7 +6312,7 @@
     </row>
     <row r="44" spans="1:34" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="211" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B44" s="212"/>
       <c r="C44" s="213"/>
@@ -8459,7 +8459,7 @@
     </row>
     <row r="91" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="132" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B91" s="133"/>
       <c r="C91" s="118"/>
@@ -9623,7 +9623,7 @@
     </row>
     <row r="117" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="131" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="B117" s="121"/>
       <c r="C117" s="122"/>
@@ -9787,7 +9787,7 @@
     </row>
     <row r="121" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="68" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B121" s="97" t="s">
         <v>155</v>
@@ -10139,7 +10139,7 @@
     </row>
     <row r="129" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B129" s="97" t="s">
         <v>171</v>
@@ -10563,7 +10563,7 @@
     </row>
     <row r="139" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="131" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B139" s="121"/>
       <c r="C139" s="122"/>
@@ -11906,7 +11906,7 @@
     <row r="170" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="171" spans="1:34" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="262" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B171" s="185"/>
       <c r="C171" s="118"/>
@@ -11944,7 +11944,7 @@
     </row>
     <row r="172" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="68" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B172" s="97" t="s">
         <v>169</v>
@@ -11988,7 +11988,7 @@
     </row>
     <row r="173" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="68" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B173" s="97" t="s">
         <v>169</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="174" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="68" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B174" s="97" t="s">
         <v>155</v>
@@ -12120,7 +12120,7 @@
     </row>
     <row r="176" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="68" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B176" s="97" t="s">
         <v>160</v>
@@ -12208,7 +12208,7 @@
     </row>
     <row r="178" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="68" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B178" s="97" t="s">
         <v>166</v>
@@ -12252,7 +12252,7 @@
     </row>
     <row r="179" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="68" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B179" s="97" t="s">
         <v>164</v>
@@ -12384,7 +12384,7 @@
     </row>
     <row r="182" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B182" s="97" t="s">
         <v>167</v>
@@ -12428,7 +12428,7 @@
     </row>
     <row r="183" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B183" s="97" t="s">
         <v>163</v>
@@ -12472,7 +12472,7 @@
     </row>
     <row r="184" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B184" s="97" t="s">
         <v>179</v>
@@ -12500,7 +12500,7 @@
       <c r="W184" s="173"/>
       <c r="X184" s="174"/>
       <c r="Y184" s="174" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Z184" s="66"/>
       <c r="AA184" s="39"/>
@@ -12514,10 +12514,10 @@
     </row>
     <row r="185" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B185" s="97" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C185" s="68"/>
       <c r="D185" s="40"/>
@@ -12541,7 +12541,7 @@
       <c r="V185" s="175"/>
       <c r="W185" s="173"/>
       <c r="X185" s="174" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Y185" s="174"/>
       <c r="Z185" s="66"/>
@@ -12600,7 +12600,7 @@
     </row>
     <row r="187" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="68" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B187" s="97" t="s">
         <v>168</v>
@@ -12644,7 +12644,7 @@
     </row>
     <row r="188" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="68" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B188" s="97" t="s">
         <v>162</v>
@@ -12688,7 +12688,7 @@
     </row>
     <row r="189" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B189" s="97" t="s">
         <v>161</v>
@@ -12732,7 +12732,7 @@
     </row>
     <row r="190" spans="1:34" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B190" s="97" t="s">
         <v>165</v>
@@ -12812,7 +12812,7 @@
     </row>
     <row r="192" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="284" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N192" s="1" t="s">
         <v>287</v>
@@ -12897,7 +12897,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>98</v>
@@ -13175,7 +13175,7 @@
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
       <c r="C13" s="40" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
@@ -13188,7 +13188,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>